<commit_message>
Comments are PD updates and Arch
</commit_message>
<xml_diff>
--- a/Jamica/Feedback.xlsx
+++ b/Jamica/Feedback.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="75">
   <si>
     <t>Author</t>
   </si>
@@ -138,6 +138,144 @@
   </si>
   <si>
     <t>The behairos that use this feactures are not enumerated</t>
+  </si>
+  <si>
+    <t>Functionality List</t>
+  </si>
+  <si>
+    <t>LED Indicator:"- Used to display system states
+            States: Normal, Sleep, Recording (respective to colors above)"</t>
+  </si>
+  <si>
+    <t>This describes behavior and so should be moved to the state Product States section</t>
+  </si>
+  <si>
+    <t>5f57365</t>
+  </si>
+  <si>
+    <t>Systems State missing LED color</t>
+  </si>
+  <si>
+    <t>Add respective colors</t>
+  </si>
+  <si>
+    <t>Still not removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sparate System Block Characteristic from implementation. For example you use the Raspbeery Pi Zero in the project but what if you used a different processor next time. What are the characteristics of both processors that you must have. </t>
+  </si>
+  <si>
+    <t>See Wearable Embedded Camera Functionality List MK Comments.txt to see how I separated the implementation out from the characteristics</t>
+  </si>
+  <si>
+    <t>Flow Diagram</t>
+  </si>
+  <si>
+    <t>Hardware Block Diagram</t>
+  </si>
+  <si>
+    <t>See The Flow Daigram Grammar and block digram for notes</t>
+  </si>
+  <si>
+    <t>Signal flow needs to be updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siganl flow needs to be updated </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We talked about this on Monday. </t>
+  </si>
+  <si>
+    <t>Event: Device is idle for 5 minutes
+           1. Device goes to power saving, sleep mode</t>
+  </si>
+  <si>
+    <t>This is how you get into the sleep state not an event that happens in it. Move this to the states where the event can happen</t>
+  </si>
+  <si>
+    <t>Initial State: Shutdown
+      Event: Power button is held for 5 seconds
+           1. Device powers off/ goes to shutdown state</t>
+  </si>
+  <si>
+    <t>Event: Power button is pressed while in shutdown state
+           1. Device powers on to normal state</t>
+  </si>
+  <si>
+    <t>Yes :) this is an event that happen in this state and casues a state transistion</t>
+  </si>
+  <si>
+    <t>How do you get out of the Sleep State</t>
+  </si>
+  <si>
+    <t>Normal State: What happens when you hit the puase button?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Event: Processor is on, charger off </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> this is not an event. What do you mean by this? </t>
+    </r>
+  </si>
+  <si>
+    <t>Good enumeration of battery and system states</t>
+  </si>
+  <si>
+    <t>Behavior Description</t>
+  </si>
+  <si>
+    <t>Product Architecture</t>
+  </si>
+  <si>
+    <t>Needs to be filled out</t>
+  </si>
+  <si>
+    <t>Let me know if you have questions about this</t>
+  </si>
+  <si>
+    <t>Major Components BOM</t>
+  </si>
+  <si>
+    <t>Rename the sheet to you project</t>
+  </si>
+  <si>
+    <t>If you adpat things you must update all the old information otherwise it will be confusing</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 16V X7R 0603
+RES SMD 1.1K OHM 1% 1/10W 0603
+RES SMD 100K OHM 1% 1/10W 0603
+THERMISTOR 10K OHM NTC 0402 SMD
+RES SMD 10K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>Remove columes that do not match your parts</t>
+  </si>
+  <si>
+    <t>Device
+PN001
+PN002
+PN003
+PN004
+PN005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What do these numbers come from? </t>
+  </si>
+  <si>
+    <t>MFG_PART_NUMBER
+LP503035</t>
+  </si>
+  <si>
+    <t>If there is not manufacture part number that is fine. Just fill out the vendor part number</t>
   </si>
 </sst>
 </file>
@@ -147,7 +285,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,6 +338,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -218,7 +363,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -270,8 +415,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -300,8 +457,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -327,6 +494,12 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -352,6 +525,12 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -681,20 +860,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="9" customWidth="1"/>
-    <col min="4" max="4" width="55" style="10" customWidth="1"/>
-    <col min="5" max="5" width="66.5" style="10" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.1640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="67.1640625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="59.5" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -749,274 +930,678 @@
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="H6" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" ht="32">
+      <c r="A8" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>16</v>
       </c>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:8" ht="64">
-      <c r="A9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>29</v>
       </c>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="32">
-      <c r="A11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" ht="48">
+      <c r="A11" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>19</v>
       </c>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:8" ht="48">
-      <c r="A12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:8" ht="32">
-      <c r="A13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="9" t="s">
+      <c r="H13" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="32">
+      <c r="A14" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="9" t="s">
+      <c r="H14" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="32">
+      <c r="A15" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>23</v>
       </c>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" ht="64">
-      <c r="A16" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="48">
-      <c r="A17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="9" t="s">
+      <c r="H16" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="48">
+      <c r="A17" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="64">
-      <c r="A18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="9" t="s">
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" ht="64">
+      <c r="A18" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="32">
-      <c r="A19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="9" t="s">
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" ht="32">
+      <c r="A19" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="E19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="F19" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="9" t="s">
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="E20" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="32">
-      <c r="A21" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="9" t="s">
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:7" ht="32">
+      <c r="A21" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="E21" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="F21" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="9" t="s">
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" ht="32">
+      <c r="A22" s="13">
+        <v>42882</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="D22" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>36</v>
+      </c>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" ht="80">
+      <c r="A23" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="96">
+      <c r="A25" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="48">
+      <c r="A28" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="64">
+      <c r="A29" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="48">
+      <c r="A30" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="32">
+      <c r="A32" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="32">
+      <c r="A33" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="32">
+      <c r="A34" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="32">
+      <c r="A36" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="80">
+      <c r="A37" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="96">
+      <c r="A38" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="96">
+      <c r="A39" s="13">
+        <v>42892</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>